<commit_message>
Mengubah Task.xlsx dan menambahkan file h3h3.txt
</commit_message>
<xml_diff>
--- a/Excel/Task.xlsx
+++ b/Excel/Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABUBAKAR\Desktop\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C9FE4C-A35C-4409-AE0D-D4FD2ABEC581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F76E23-F86C-418C-9DC8-7F49C8F450D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Honda</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Honda03</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>KIA</t>
   </si>
 </sst>
 </file>
@@ -351,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,6 +380,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel sm text berubah
h3h3.txt
-hehe3
+hehe4
+hehe5

excel
+BMM
+Hyundai
</commit_message>
<xml_diff>
--- a/Excel/Task.xlsx
+++ b/Excel/Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABUBAKAR\Desktop\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F76E23-F86C-418C-9DC8-7F49C8F450D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95712D8-1328-461B-8071-7BA3B342C7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Honda</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>KIA</t>
+  </si>
+  <si>
+    <t>BMM</t>
+  </si>
+  <si>
+    <t>Nissan</t>
   </si>
 </sst>
 </file>
@@ -357,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,6 +396,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>